<commit_message>
Fix filtering of students in generate_excel_students function
</commit_message>
<xml_diff>
--- a/static/course-students-excel/2559206.xlsx
+++ b/static/course-students-excel/2559206.xlsx
@@ -459,7 +459,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F32"/>
+  <dimension ref="A2:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -941,27 +941,27 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1035441617</t>
+          <t>1000921490</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>JHON EDISON LONDOÑO CARVAJAL</t>
+          <t>JUAN SEBASTIAN TAMAYO TORO</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>3192196594</t>
+          <t>3013567242</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>jhonedi990223@gmail.com</t>
+          <t>jstamayotoro@hotmail.com</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>TRASLADADO</t>
+          <t>EN FORMACION</t>
         </is>
       </c>
     </row>
@@ -973,22 +973,22 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>1000921490</t>
+          <t>1151935314</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>JUAN SEBASTIAN TAMAYO TORO</t>
+          <t>JULIAN ANDRES CARREÑO TEJADA</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>3013567242</t>
+          <t>3158099913</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>jstamayotoro@hotmail.com</t>
+          <t>julianctsistemas@gmail.com</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1005,22 +1005,22 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>1151935314</t>
+          <t>1035129796</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>JULIAN ANDRES CARREÑO TEJADA</t>
+          <t>MARCELA MORALES MORENO</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>3158099913</t>
+          <t>3214935688</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>julianctsistemas@gmail.com</t>
+          <t>marcelamorales1808@gmail.com</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1037,22 +1037,22 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1035129796</t>
+          <t>1000438854</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>MARCELA MORALES MORENO</t>
+          <t>MARIANA GRANADOS SIERRA</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>3214935688</t>
+          <t>3218505800</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>marcelamorales1808@gmail.com</t>
+          <t>marianagranados201@gmail.com</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1069,22 +1069,22 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>1000438854</t>
+          <t>1001234788</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>MARIANA GRANADOS SIERRA</t>
+          <t>MARTIN ALEJANDRO PINZON CALDERON</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>3218505800</t>
+          <t>3218821649</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>marianagranados201@gmail.com</t>
+          <t>mpinzonc07@gmail.com</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1101,22 +1101,22 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1001234788</t>
+          <t>1020495400</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>MARTIN ALEJANDRO PINZON CALDERON</t>
+          <t>OSCAR ALBERTO TORRES VALLADALES</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>3218821649</t>
+          <t>3046531816</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>mpinzonc07@gmail.com</t>
+          <t>oscartorres990926@outlook.com</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1133,22 +1133,22 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1020495400</t>
+          <t>1014478296</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>OSCAR ALBERTO TORRES VALLADALES</t>
+          <t>PAULA ALEJANDRA NIÑO BUITRAGO</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>3046531816</t>
+          <t>3007315538</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>oscartorres990926@outlook.com</t>
+          <t>paulanb.03@gmail.com</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1165,22 +1165,22 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1014478296</t>
+          <t>1035442288</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>PAULA ALEJANDRA NIÑO BUITRAGO</t>
+          <t>SANTIAGO SOSA CADAVID</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>3007315538</t>
+          <t>3017655840</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>paulanb.03@gmail.com</t>
+          <t>santi4586sosa@gmail.com</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1197,22 +1197,22 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1035442288</t>
+          <t>1048046418</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>SANTIAGO SOSA CADAVID</t>
+          <t>SIMON RUIZ GARCIA</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>3017655840</t>
+          <t>3504335065</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>santi4586sosa@gmail.com</t>
+          <t>simon01ruiz@gmail.com</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1229,22 +1229,22 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>1048046418</t>
+          <t>1001227509</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>SIMON RUIZ GARCIA</t>
+          <t>SIMON ESTEBAN ZULETA HENAO</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>3504335065</t>
+          <t>3217212128</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>simon01ruiz@gmail.com</t>
+          <t>simonzh1407@gmail.com</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1261,57 +1261,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>1001227509</t>
+          <t>1018226926</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>SIMON ESTEBAN ZULETA HENAO</t>
+          <t>VALERIA CARMONA SUAREZ</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>3217212128</t>
+          <t>3112962479</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>simonzh1407@gmail.com</t>
+          <t>valeriazaarez.12@gmail.com</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
-        <is>
-          <t>EN FORMACION</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>1018226926</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>VALERIA CARMONA SUAREZ</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>3112962479</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>valeriazaarez.12@gmail.com</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
         <is>
           <t>EN FORMACION</t>
         </is>

</xml_diff>